<commit_message>
adicionando projeto sobre tratamento, análise e insghts dos dados com inteligência artificial
</commit_message>
<xml_diff>
--- a/planilhas-dinamicas/assets/documents/planilha-dinamica.xlsx
+++ b/planilhas-dinamicas/assets/documents/planilha-dinamica.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr hidePivotFieldList="1"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12825" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="28800" windowHeight="12825"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="Economias" sheetId="4" state="hidden" r:id="rId2"/>
-    <sheet name="Controller" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Economias" sheetId="4" r:id="rId2"/>
+    <sheet name="Controller" sheetId="2" r:id="rId3"/>
     <sheet name="Dashboard" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
@@ -591,7 +591,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -757,12 +757,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1034,28 +1028,28 @@
     <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7162,7 +7156,7 @@
   </sheetPr>
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -8882,7 +8876,7 @@
   </sheetPr>
   <dimension ref="N5:R19"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
       <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>

</xml_diff>